<commit_message>
Changes in keyword file
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Creator_Platform.xlsx
+++ b/src/test/java/com/genvideo/xls/Creator_Platform.xlsx
@@ -825,10 +825,10 @@
     <t>genvideotest1078@gmail.com</t>
   </si>
   <si>
-    <t>genvideotest1196@gmail.com</t>
-  </si>
-  <si>
-    <t>genvideotest1197@gmail.com</t>
+    <t>genvideotest1198@gmail.com</t>
+  </si>
+  <si>
+    <t>genvideotest1199@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -6669,8 +6669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R2" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Reports commited for 20th May 2016
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Creator_Platform.xlsx
+++ b/src/test/java/com/genvideo/xls/Creator_Platform.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2563" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="269">
   <si>
     <t>TCID</t>
   </si>
@@ -825,17 +825,16 @@
     <t>genvideotest1078@gmail.com</t>
   </si>
   <si>
-    <t>genvideotest1210@gmail.com</t>
-  </si>
-  <si>
-    <t>genvideotest1209@gmail.com</t>
+    <t>genvideotest1215@gmail.com</t>
+  </si>
+  <si>
+    <t>genvideotest1216@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1451,10 +1450,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="23.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="37.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="18.28515625" collapsed="true"/>
-    <col min="4" max="16384" style="2" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="23.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="8.85546875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1500,30 +1499,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R108"/>
   <sheetViews>
-    <sheetView topLeftCell="H84" workbookViewId="0">
-      <selection activeCell="H104" sqref="H104"/>
+    <sheetView topLeftCell="B94" workbookViewId="0">
+      <selection activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="20.28515625" collapsed="true"/>
-    <col min="2" max="2" style="2" width="8.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="47.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="20.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="36.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="2" width="24.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="8.62890625" collapsed="true"/>
-    <col min="18" max="16384" style="2" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="20.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.85546875" style="2" collapsed="1"/>
+    <col min="3" max="3" width="47.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="255" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="16384" width="8.85546875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -6678,20 +6670,20 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="7" width="28.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="7" width="25.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="7" width="33.28515625" collapsed="true"/>
-    <col min="4" max="14" customWidth="true" style="7" width="25.140625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="7" width="15.42578125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="7" width="17.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="7" width="9.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="7" width="6.3984375" collapsed="true"/>
-    <col min="19" max="16384" style="7" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="28.28515625" style="7" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.140625" style="7" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.28515625" style="7" customWidth="1" collapsed="1"/>
+    <col min="4" max="14" width="25.140625" style="7" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.42578125" style="7" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17" style="7" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="9.42578125" style="7" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="255" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="16384" width="8.85546875" style="7" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -6752,13 +6744,13 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>58</v>
@@ -7290,10 +7282,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="33.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="1" max="1" width="33.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
reports commited for 25th july
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Creator_Platform.xlsx
+++ b/src/test/java/com/genvideo/xls/Creator_Platform.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2563" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2562" uniqueCount="270">
   <si>
     <t>TCID</t>
   </si>
@@ -826,148 +826,18 @@
   </si>
   <si>
     <t>FAIL -- Not able to click on ButtonElement is not currently visible and so may not be interacted with
-Command duration or timeout: 20.07 seconds
+Command duration or timeout: 120.04 seconds
 Build info: version: '2.53.0', revision: '35ae25b', time: '2016-03-15 17:00:58'
 System info: host: 'pclap-002', ip: '172.16.146.33', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
 Driver info: org.openqa.selenium.firefox.FirefoxDriver
 Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=45.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 5f070305-64d0-4561-bbbb-28ef1b3645e2</t>
-  </si>
-  <si>
-    <t>FAIL Unable to write Element is not currently visible and so may not be interacted with
-Command duration or timeout: 20.11 seconds
-Build info: version: '2.53.0', revision: '35ae25b', time: '2016-03-15 17:00:58'
-System info: host: 'pclap-002', ip: '172.16.146.33', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=45.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 5f070305-64d0-4561-bbbb-28ef1b3645e2</t>
-  </si>
-  <si>
-    <t>FAIL -- Not able to click on linkElement is not currently visible and so may not be interacted with
-Command duration or timeout: 20.11 seconds
-Build info: version: '2.53.0', revision: '35ae25b', time: '2016-03-15 17:00:58'
-System info: host: 'pclap-002', ip: '172.16.146.33', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=45.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 5f070305-64d0-4561-bbbb-28ef1b3645e2</t>
-  </si>
-  <si>
-    <t>FAIL -- Not able to click on linkElement is not currently visible and so may not be interacted with
-Command duration or timeout: 20.12 seconds
-Build info: version: '2.53.0', revision: '35ae25b', time: '2016-03-15 17:00:58'
-System info: host: 'pclap-002', ip: '172.16.146.33', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=45.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 5f070305-64d0-4561-bbbb-28ef1b3645e2</t>
-  </si>
-  <si>
-    <t>FAIL -- Not able to click on linkElement is not currently visible and so may not be interacted with
-Command duration or timeout: 20.07 seconds
-Build info: version: '2.53.0', revision: '35ae25b', time: '2016-03-15 17:00:58'
-System info: host: 'pclap-002', ip: '172.16.146.33', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=45.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 5f070305-64d0-4561-bbbb-28ef1b3645e2</t>
-  </si>
-  <si>
-    <t>FAIL Unable to write Element is not currently visible and so may not be interacted with
-Command duration or timeout: 20.08 seconds
-Build info: version: '2.53.0', revision: '35ae25b', time: '2016-03-15 17:00:58'
-System info: host: 'pclap-002', ip: '172.16.146.33', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=45.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 5f070305-64d0-4561-bbbb-28ef1b3645e2</t>
-  </si>
-  <si>
-    <t>FAIL Unable to write Element is not currently visible and so may not be interacted with
-Command duration or timeout: 20.02 seconds
-Build info: version: '2.53.0', revision: '35ae25b', time: '2016-03-15 17:00:58'
-System info: host: 'pclap-002', ip: '172.16.146.33', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=45.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 5f070305-64d0-4561-bbbb-28ef1b3645e2</t>
-  </si>
-  <si>
-    <t>FAIL -- Not able to click on linkUnable to locate element: {"method":"xpath","selector":"html/body/div[2]/div/div/div/div/div/div[2]/div[4]/div/div[2]/ng-form/div[4]/div/tags-search/div/div/ul/li[3]"}
-Command duration or timeout: 20.12 seconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: '2.53.0', revision: '35ae25b', time: '2016-03-15 17:00:58'
-System info: host: 'pclap-002', ip: '172.16.146.33', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=45.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 5f070305-64d0-4561-bbbb-28ef1b3645e2
-*** Element info: {Using=xpath, value=html/body/div[2]/div/div/div/div/div/div[2]/div[4]/div/div[2]/ng-form/div[4]/div/tags-search/div/div/ul/li[3]}</t>
-  </si>
-  <si>
-    <t>FAIL -- Not able to click on linkElement is not currently visible and so may not be interacted with
-Command duration or timeout: 20.09 seconds
-Build info: version: '2.53.0', revision: '35ae25b', time: '2016-03-15 17:00:58'
-System info: host: 'pclap-002', ip: '172.16.146.33', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=45.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 5f070305-64d0-4561-bbbb-28ef1b3645e2</t>
-  </si>
-  <si>
-    <t>FAIL -- Not able to click on linkElement is not currently visible and so may not be interacted with
-Command duration or timeout: 20.02 seconds
-Build info: version: '2.53.0', revision: '35ae25b', time: '2016-03-15 17:00:58'
-System info: host: 'pclap-002', ip: '172.16.146.33', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=45.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 5f070305-64d0-4561-bbbb-28ef1b3645e2</t>
-  </si>
-  <si>
-    <t>FAIL -- Not able to click on linkElement is not currently visible and so may not be interacted with
-Command duration or timeout: 20.06 seconds
-Build info: version: '2.53.0', revision: '35ae25b', time: '2016-03-15 17:00:58'
-System info: host: 'pclap-002', ip: '172.16.146.33', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=45.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 5f070305-64d0-4561-bbbb-28ef1b3645e2</t>
-  </si>
-  <si>
-    <t>FAIL -- Not able to click on linkElement is not currently visible and so may not be interacted with
-Command duration or timeout: 20.08 seconds
-Build info: version: '2.53.0', revision: '35ae25b', time: '2016-03-15 17:00:58'
-System info: host: 'pclap-002', ip: '172.16.146.33', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=45.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 5f070305-64d0-4561-bbbb-28ef1b3645e2</t>
-  </si>
-  <si>
-    <t>FAIL -- Not able to click on linkElement is not currently visible and so may not be interacted with
-Command duration or timeout: 20.05 seconds
-Build info: version: '2.53.0', revision: '35ae25b', time: '2016-03-15 17:00:58'
-System info: host: 'pclap-002', ip: '172.16.146.33', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=45.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 5f070305-64d0-4561-bbbb-28ef1b3645e2</t>
-  </si>
-  <si>
-    <t>FAIL -- Not able to click on linkElement is not currently visible and so may not be interacted with
-Command duration or timeout: 20.10 seconds
-Build info: version: '2.53.0', revision: '35ae25b', time: '2016-03-15 17:00:58'
-System info: host: 'pclap-002', ip: '172.16.146.33', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=45.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 5f070305-64d0-4561-bbbb-28ef1b3645e2</t>
-  </si>
-  <si>
-    <t>FAIL -- Not able to click on linkUnable to locate element: {"method":"xpath","selector":"html/body/header/nav/div[2]/ul[1]/li[3]/a"}
-Command duration or timeout: 20.05 seconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: '2.53.0', revision: '35ae25b', time: '2016-03-15 17:00:58'
-System info: host: 'pclap-002', ip: '172.16.146.33', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=45.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 5f070305-64d0-4561-bbbb-28ef1b3645e2
-*** Element info: {Using=xpath, value=html/body/header/nav/div[2]/ul[1]/li[3]/a}</t>
-  </si>
-  <si>
-    <t>genvideotest1221@gmail.com</t>
-  </si>
-  <si>
-    <t>genvideotest1222@gmail.com</t>
+Session ID: 55cf97b0-95bb-41c6-9038-04c87adcb7a9</t>
+  </si>
+  <si>
+    <t>genvideotest1229@gmail.com</t>
+  </si>
+  <si>
+    <t>genvideotest1230@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -6817,7 +6687,7 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6891,13 +6761,13 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
Reports committed for 27 May 2016
</commit_message>
<xml_diff>
--- a/src/test/java/com/genvideo/xls/Creator_Platform.xlsx
+++ b/src/test/java/com/genvideo/xls/Creator_Platform.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2562" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2560" uniqueCount="269">
   <si>
     <t>TCID</t>
   </si>
@@ -825,19 +825,10 @@
     <t>genvideotest1078@gmail.com</t>
   </si>
   <si>
-    <t>FAIL -- Not able to click on ButtonElement is not currently visible and so may not be interacted with
-Command duration or timeout: 120.04 seconds
-Build info: version: '2.53.0', revision: '35ae25b', time: '2016-03-15 17:00:58'
-System info: host: 'pclap-002', ip: '172.16.146.33', os.name: 'Windows 7', os.arch: 'amd64', os.version: '6.1', java.version: '1.8.0_65'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=45.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 55cf97b0-95bb-41c6-9038-04c87adcb7a9</t>
-  </si>
-  <si>
-    <t>genvideotest1229@gmail.com</t>
-  </si>
-  <si>
-    <t>genvideotest1230@gmail.com</t>
+    <t>genvideotest1233@gmail.com</t>
+  </si>
+  <si>
+    <t>genvideotest1234@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -6687,7 +6678,7 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6761,13 +6752,13 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>58</v>

</xml_diff>